<commit_message>
Finalizado o projeto de TDD
</commit_message>
<xml_diff>
--- a/TestaData.xlsx
+++ b/TestaData.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renan.silva\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renan.silva\eclipse-workspace\tdd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841967F6-851E-472A-B3A0-CE3E1DD44801}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569E108D-AA7B-4E5A-9540-5A2C0F72DD3E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{34EB691A-787E-44EA-9E71-78C542212629}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{34EB691A-787E-44EA-9E71-78C542212629}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="CadastroFalha" sheetId="1" r:id="rId1"/>
+    <sheet name="CadastroSucesso" sheetId="4" r:id="rId2"/>
+    <sheet name="Pesquisa" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
   <si>
     <t>NomeDeUsuario</t>
   </si>
   <si>
-    <t>RenanMarcos</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -97,6 +96,24 @@
   </si>
   <si>
     <t>CodigoPostal</t>
+  </si>
+  <si>
+    <t>barraDePesquisa</t>
+  </si>
+  <si>
+    <t>HP ELITEPAD 1000 G2 TABLET</t>
+  </si>
+  <si>
+    <t>produto inexistente</t>
+  </si>
+  <si>
+    <t>GALAXY GRAN PRIME</t>
+  </si>
+  <si>
+    <t>RenanMarcos2</t>
+  </si>
+  <si>
+    <t>RenanMarcos10</t>
   </si>
 </sst>
 </file>
@@ -120,7 +137,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,6 +147,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -162,11 +185,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -484,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC764D2F-EC9D-4DC8-A633-DA943D0481F0}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,72 +527,72 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="K2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L2" s="1">
         <v>3582180</v>
@@ -582,4 +606,143 @@
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A27493A-5BA7-49A0-B125-3F25B29CDC0B}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="1">
+        <v>3582180</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{EBCD22C1-1C40-4BA5-9E94-925A06EA9204}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{4D5AD43D-202C-4A0C-9D92-971CA1225060}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{30CD903A-F136-48D0-B579-17B2DE644E0A}"/>
+  </hyperlinks>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B43EBD39-174A-4247-A449-B004F7023FCC}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>